<commit_message>
new review and allocate
</commit_message>
<xml_diff>
--- a/src/main/resources/static/source/专家信息表.xlsx
+++ b/src/main/resources/static/source/专家信息表.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lenovo\Desktop\评审系统-分析\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\gittest\review\src\main\resources\static\source\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F7D6B4B-F581-4CAE-B523-82B04E7F0C1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E4E40C9-A86C-4C2B-9775-6DEEEBC6C69B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="35">
   <si>
     <t>工号</t>
   </si>
@@ -49,9 +49,6 @@
     <t>张旺</t>
   </si>
   <si>
-    <t>科员</t>
-  </si>
-  <si>
     <t>初级工程师</t>
   </si>
   <si>
@@ -62,9 +59,6 @@
   </si>
   <si>
     <t>张恒</t>
-  </si>
-  <si>
-    <t>工程</t>
   </si>
   <si>
     <t>000329</t>
@@ -115,14 +109,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>高级工程师</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>财务</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>单位</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -132,6 +118,19 @@
   </si>
   <si>
     <t>研究所</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>华西</t>
+  </si>
+  <si>
+    <t>华中</t>
+  </si>
+  <si>
+    <t>华东</t>
+  </si>
+  <si>
+    <t>科员</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -538,7 +537,7 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -567,10 +566,10 @@
         <v>4</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="G1" s="11" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>5</v>
@@ -586,19 +585,21 @@
       <c r="B2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="E2" s="10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="G2" s="10"/>
+        <v>30</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="H2" s="2">
         <v>15991252344</v>
       </c>
@@ -608,24 +609,26 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>14</v>
+      <c r="E3" s="10" t="s">
+        <v>27</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="G3" s="10"/>
+        <v>30</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="H3" s="2">
         <v>13659196637</v>
       </c>
@@ -635,24 +638,26 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>14</v>
+      <c r="E4" s="10" t="s">
+        <v>27</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="G4" s="10"/>
+        <v>30</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="H4" s="2">
         <v>18591981653</v>
       </c>
@@ -662,24 +667,26 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>34</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>10</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="G5" s="10"/>
+        <v>30</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>33</v>
+      </c>
       <c r="H5" s="2">
         <v>15319783096</v>
       </c>
@@ -689,24 +696,26 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="F6" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="G6" s="10"/>
+        <v>30</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>32</v>
+      </c>
       <c r="H6" s="3">
         <v>17391986497</v>
       </c>
@@ -716,24 +725,26 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="F7" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="G7" s="10"/>
+      <c r="G7" s="10" t="s">
+        <v>33</v>
+      </c>
       <c r="H7" s="3">
         <v>13572081862</v>
       </c>
@@ -743,9 +754,18 @@
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <dataValidations count="1">
+  <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G7" xr:uid="{1FCF1F30-49E4-4DD3-A6C3-82AA123A811A}">
       <formula1>"华东,华西,华中,华北,华南"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D7" xr:uid="{7B46BF7F-16F4-482C-B1D0-AFDFCD64FEBF}">
+      <formula1>"初级工程师,中级工程师,高级工程师"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E7" xr:uid="{79A55A14-75D0-4D31-8AEB-ACB864DC88F1}">
+      <formula1>"工程,财务,地质"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C7" xr:uid="{8FA3674B-0B14-4905-BB73-2B979E81C1CF}">
+      <formula1>"科员,副科,正科,副处,正处"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>